<commit_message>
[HF-92][Zhen Tang] feat: update the chw import template
</commit_message>
<xml_diff>
--- a/public/static/template/import_chw.xlsx
+++ b/public/static/template/import_chw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ztang/workspace/unc/src/visit-link-admin-web/public/static/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C7A1A1-BDF1-C144-9EC1-7C6300F0138D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308894B3-86A2-1545-9C51-A0560063E4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14680" yWindow="2180" windowWidth="22360" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27500" yWindow="1900" windowWidth="25800" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baby Roster" sheetId="1" r:id="rId1"/>
@@ -47,17 +47,17 @@
 2.校验：表格内不重复；后台内不重复</t>
   </si>
   <si>
-    <t>1.必填
-2.格式：省/市/区/街道或乡镇
-3.街道或乡镇最多只能添加3个，添加1个以上区域需用英文","隔开</t>
-  </si>
-  <si>
     <t>1. 必填
 2. 社区工作者电话:5-20位手机号码</t>
   </si>
   <si>
     <t>1.必填
 2.校验：不能超过50个字符，不允许特殊字符</t>
+  </si>
+  <si>
+    <t>1.必填
+2.格式：省/市/区/街道或乡镇
+3.街道或乡镇最多只能添加3个，添加1个以上区域需用英文";"隔开</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1307,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.75" customHeight="1"/>
@@ -1367,16 +1367,16 @@
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="88" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>6</v>

</xml_diff>